<commit_message>
Added surefireplugin and firefox browser support
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myFIles\Github\Frameworks\ngframework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\ngframework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EBDBD0-D341-4579-BC0B-5362782F73B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B38D12-C01F-4114-B025-59EA80200682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" activeTab="1" xr2:uid="{AFC5DEC4-B811-4934-BDEB-F9BD32BBFB86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AFC5DEC4-B811-4934-BDEB-F9BD32BBFB86}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>testname</t>
   </si>
@@ -104,6 +102,12 @@
   </si>
   <si>
     <t>brendon</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -477,10 +481,10 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -545,20 +549,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F47D3E-0080-4D4B-8CF4-0C3A5FC11DA7}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -566,16 +570,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -583,16 +590,19 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -600,30 +610,36 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -631,16 +647,19 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,9 +667,12 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Disabled test report mailing
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\ngframework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B38D12-C01F-4114-B025-59EA80200682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAF8B95-C122-4B9C-B498-C171A5998C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AFC5DEC4-B811-4934-BDEB-F9BD32BBFB86}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>testname</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>admin123</t>
-  </si>
-  <si>
-    <t>admin</t>
   </si>
   <si>
     <t>Admin</t>
@@ -552,7 +549,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,7 +567,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -590,16 +587,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -610,16 +607,16 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -630,13 +627,13 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -647,16 +644,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -667,13 +664,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>